<commit_message>
Change led package to 3mm
</commit_message>
<xml_diff>
--- a/CaptorBoard.xlsx
+++ b/CaptorBoard.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr date1904="1" showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CaptorBoard.csv" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="140">
   <si>
     <t>Reference</t>
   </si>
@@ -376,9 +376,6 @@
     <t>LED</t>
   </si>
   <si>
-    <t>Gide lumiere</t>
-  </si>
-  <si>
     <t>Foot print</t>
   </si>
   <si>
@@ -412,9 +409,6 @@
     <t>Diode-MiniMELF_Standard</t>
   </si>
   <si>
-    <t>LED-1206</t>
-  </si>
-  <si>
     <t>Fuseholder5x20_horiz_SemiClosed_Casing10x25mm</t>
   </si>
   <si>
@@ -443,6 +437,9 @@
   </si>
   <si>
     <t>For 2 board</t>
+  </si>
+  <si>
+    <t>LED-3mm</t>
   </si>
 </sst>
 </file>
@@ -1205,7 +1202,7 @@
         <v>96</v>
       </c>
       <c r="B29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C29" t="s">
         <v>11</v>
@@ -1216,7 +1213,7 @@
         <v>97</v>
       </c>
       <c r="B30" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C30" t="s">
         <v>11</v>
@@ -1502,7 +1499,7 @@
         <v>94</v>
       </c>
       <c r="B56" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C56" t="s">
         <v>95</v>
@@ -1529,10 +1526,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1557,11 +1557,11 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1571,7 +1571,7 @@
         <v>113</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>114</v>
@@ -1583,7 +1583,7 @@
         <v>115</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>114</v>
@@ -1592,7 +1592,7 @@
         <v>116</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>114</v>
@@ -1606,7 +1606,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -1645,7 +1645,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -1660,22 +1660,22 @@
         <v>1</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" ref="G4:G35" si="0">ROUNDUP(C4/F4,0)*F4</f>
+        <f t="shared" ref="G4:G34" si="0">ROUNDUP(C4/F4,0)*F4</f>
         <v>1</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" ref="H4:H35" si="1">G4*E4</f>
+        <f t="shared" ref="H4:H34" si="1">G4*E4</f>
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="I4" s="1">
         <v>2</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" ref="J4:J35" si="2">ROUNDUP(($C4*I4)/$F4,0)*$F4</f>
+        <f t="shared" ref="J4:J34" si="2">ROUNDUP(($C4*I4)/$F4,0)*$F4</f>
         <v>2</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" ref="K4:K35" si="3">$E4*J4</f>
+        <f t="shared" ref="K4:K34" si="3">$E4*J4</f>
         <v>9.1999999999999998E-2</v>
       </c>
     </row>
@@ -1684,7 +1684,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -1723,7 +1723,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C6" s="1">
         <v>7</v>
@@ -1762,7 +1762,7 @@
         <v>103</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -1801,7 +1801,7 @@
         <v>56</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -1840,7 +1840,7 @@
         <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -1879,7 +1879,7 @@
         <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C10" s="1">
         <v>2</v>
@@ -1918,7 +1918,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C11" s="1">
         <v>2</v>
@@ -1954,10 +1954,10 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C12" s="1">
         <v>2</v>
@@ -1996,7 +1996,7 @@
         <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
@@ -2035,7 +2035,7 @@
         <v>87</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -2074,7 +2074,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C15" s="1">
         <v>2</v>
@@ -2113,16 +2113,16 @@
         <v>117</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="C16" s="1">
         <v>5</v>
       </c>
       <c r="D16" s="1">
-        <v>2099247</v>
+        <v>1142502</v>
       </c>
       <c r="E16" s="1">
-        <v>9.2100000000000001E-2</v>
+        <v>0.106</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -2133,7 +2133,7 @@
       </c>
       <c r="H16" s="1">
         <f t="shared" si="1"/>
-        <v>0.46050000000000002</v>
+        <v>0.53</v>
       </c>
       <c r="I16" s="1">
         <v>2</v>
@@ -2144,121 +2144,123 @@
       </c>
       <c r="K16" s="1">
         <f t="shared" si="3"/>
-        <v>0.92100000000000004</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="1" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1">
-        <v>5</v>
-      </c>
-      <c r="D17" s="1">
-        <v>3245147</v>
-      </c>
-      <c r="E17" s="1">
-        <v>0.28100000000000003</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
       <c r="F17">
         <v>1</v>
       </c>
       <c r="G17" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H17" s="1">
         <f t="shared" si="1"/>
-        <v>1.4050000000000002</v>
+        <v>0</v>
       </c>
       <c r="I17" s="1">
         <v>2</v>
       </c>
       <c r="J17" s="1">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="K17" s="1">
         <f t="shared" si="3"/>
-        <v>2.8100000000000005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="1"/>
+        <v>110</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>135</v>
+      </c>
       <c r="C18" s="1">
         <v>1</v>
       </c>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
+      <c r="D18" s="1">
+        <v>1022251</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.106</v>
+      </c>
       <c r="F18">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G18" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H18" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.06</v>
       </c>
       <c r="I18" s="1">
         <v>2</v>
       </c>
       <c r="J18" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K18" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C19" s="1">
         <v>1</v>
       </c>
       <c r="D19" s="1">
-        <v>1022251</v>
+        <v>2471682</v>
       </c>
       <c r="E19" s="1">
-        <v>0.106</v>
+        <v>0.64800000000000002</v>
       </c>
       <c r="F19">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G19" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H19" s="1">
         <f t="shared" si="1"/>
-        <v>1.06</v>
+        <v>0.64800000000000002</v>
       </c>
       <c r="I19" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J19" s="1">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="K19" s="1">
         <f t="shared" si="3"/>
-        <v>1.06</v>
+        <v>0.64800000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="1" t="s">
-        <v>107</v>
+        <v>130</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>131</v>
@@ -2267,87 +2269,81 @@
         <v>1</v>
       </c>
       <c r="D20" s="1">
-        <v>2471682</v>
+        <v>1123121</v>
       </c>
       <c r="E20" s="1">
-        <v>0.64800000000000002</v>
+        <v>0.22800000000000001</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G20" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H20" s="1">
         <f t="shared" si="1"/>
-        <v>0.64800000000000002</v>
+        <v>2.2800000000000002</v>
       </c>
       <c r="I20" s="1">
         <v>1</v>
       </c>
       <c r="J20" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K20" s="1">
         <f t="shared" si="3"/>
-        <v>0.64800000000000002</v>
+        <v>2.2800000000000002</v>
       </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>133</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B21" s="1"/>
       <c r="C21" s="1">
         <v>1</v>
       </c>
       <c r="D21" s="1">
-        <v>1123121</v>
+        <v>2058064</v>
       </c>
       <c r="E21" s="1">
-        <v>0.22800000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="F21">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G21" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H21" s="1">
         <f t="shared" si="1"/>
-        <v>2.2800000000000002</v>
+        <v>1.3</v>
       </c>
       <c r="I21" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J21" s="1">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="K21" s="1">
         <f t="shared" si="3"/>
-        <v>2.2800000000000002</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
-        <v>29</v>
+        <v>58</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1">
         <v>1</v>
       </c>
-      <c r="D22" s="1">
-        <v>2058064</v>
-      </c>
-      <c r="E22" s="1">
-        <v>1.3</v>
-      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
       <c r="F22">
         <v>1</v>
       </c>
@@ -2357,7 +2353,7 @@
       </c>
       <c r="H22" s="1">
         <f t="shared" si="1"/>
-        <v>1.3</v>
+        <v>0</v>
       </c>
       <c r="I22" s="1">
         <v>2</v>
@@ -2368,106 +2364,110 @@
       </c>
       <c r="K22" s="1">
         <f t="shared" si="3"/>
-        <v>2.6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="1" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1">
         <v>1</v>
       </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
+      <c r="D23" s="1">
+        <v>9103503</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0.51400000000000001</v>
+      </c>
       <c r="F23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G23" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H23" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.5700000000000003</v>
       </c>
       <c r="I23" s="1">
         <v>2</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K23" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2.5700000000000003</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="1" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1">
         <v>1</v>
       </c>
       <c r="D24" s="1">
-        <v>9103503</v>
+        <v>1654060</v>
       </c>
       <c r="E24" s="1">
-        <v>0.51400000000000001</v>
+        <v>0.96</v>
       </c>
       <c r="F24">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G24" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H24" s="1">
         <f t="shared" si="1"/>
-        <v>2.5700000000000003</v>
+        <v>0.96</v>
       </c>
       <c r="I24" s="1">
         <v>2</v>
       </c>
       <c r="J24" s="1">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K24" s="1">
         <f t="shared" si="3"/>
-        <v>2.5700000000000003</v>
+        <v>1.92</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>99</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" s="1">
-        <v>1654060</v>
+        <v>1021368</v>
       </c>
       <c r="E25" s="1">
-        <v>0.96</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F25">
         <v>1</v>
       </c>
       <c r="G25" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H25" s="1">
         <f t="shared" si="1"/>
-        <v>0.96</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I25" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J25" s="1">
         <f t="shared" si="2"/>
@@ -2475,96 +2475,96 @@
       </c>
       <c r="K25" s="1">
         <f t="shared" si="3"/>
-        <v>1.92</v>
+        <v>2.2000000000000002</v>
       </c>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="1" t="s">
-        <v>99</v>
+        <v>132</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1">
         <v>2</v>
       </c>
       <c r="D26" s="1">
-        <v>1021368</v>
+        <v>2445619</v>
       </c>
       <c r="E26" s="1">
-        <v>1.1000000000000001</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G26" s="1">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H26" s="1">
         <f t="shared" si="1"/>
-        <v>2.2000000000000002</v>
+        <v>2.04</v>
       </c>
       <c r="I26" s="1">
         <v>1</v>
       </c>
       <c r="J26" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K26" s="1">
         <f t="shared" si="3"/>
-        <v>2.2000000000000002</v>
+        <v>2.04</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="1" t="s">
-        <v>134</v>
+        <v>52</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" s="1">
-        <v>2445619</v>
+        <v>2102577</v>
       </c>
       <c r="E27" s="1">
-        <v>0.20399999999999999</v>
+        <v>2.77</v>
       </c>
       <c r="F27">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G27" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H27" s="1">
         <f t="shared" si="1"/>
-        <v>2.04</v>
+        <v>2.77</v>
       </c>
       <c r="I27" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J27" s="1">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="K27" s="1">
         <f t="shared" si="3"/>
-        <v>2.04</v>
+        <v>5.54</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1">
         <v>1</v>
       </c>
       <c r="D28" s="1">
-        <v>2102577</v>
+        <v>1630202</v>
       </c>
       <c r="E28" s="1">
-        <v>2.77</v>
+        <v>5.61</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -2575,7 +2575,7 @@
       </c>
       <c r="H28" s="1">
         <f t="shared" si="1"/>
-        <v>2.77</v>
+        <v>5.61</v>
       </c>
       <c r="I28" s="1">
         <v>2</v>
@@ -2586,22 +2586,22 @@
       </c>
       <c r="K28" s="1">
         <f t="shared" si="3"/>
-        <v>5.54</v>
+        <v>11.22</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1">
         <v>1</v>
       </c>
       <c r="D29" s="1">
-        <v>1630202</v>
+        <v>1778989</v>
       </c>
       <c r="E29" s="1">
-        <v>5.61</v>
+        <v>9.67</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -2612,7 +2612,7 @@
       </c>
       <c r="H29" s="1">
         <f t="shared" si="1"/>
-        <v>5.61</v>
+        <v>9.67</v>
       </c>
       <c r="I29" s="1">
         <v>2</v>
@@ -2623,22 +2623,24 @@
       </c>
       <c r="K29" s="1">
         <f t="shared" si="3"/>
-        <v>11.22</v>
+        <v>19.34</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="1"/>
+        <v>62</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>136</v>
+      </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
       <c r="D30" s="1">
-        <v>1778989</v>
+        <v>3041475</v>
       </c>
       <c r="E30" s="1">
-        <v>9.67</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="F30">
         <v>1</v>
@@ -2649,217 +2651,178 @@
       </c>
       <c r="H30" s="1">
         <f t="shared" si="1"/>
-        <v>9.67</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="I30" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J30" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K30" s="1">
         <f t="shared" si="3"/>
-        <v>19.34</v>
+        <v>1.0900000000000001</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="1" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
       </c>
       <c r="D31" s="1">
-        <v>3041475</v>
+        <v>1022255</v>
       </c>
       <c r="E31" s="1">
-        <v>1.0900000000000001</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="G31" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="H31" s="1">
         <f t="shared" si="1"/>
-        <v>1.0900000000000001</v>
+        <v>1.3800000000000001</v>
       </c>
       <c r="I31" s="1">
         <v>1</v>
       </c>
       <c r="J31" s="1">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="K31" s="1">
         <f t="shared" si="3"/>
-        <v>1.0900000000000001</v>
+        <v>1.3800000000000001</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>136</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="B32" s="1"/>
       <c r="C32" s="1">
         <v>1</v>
       </c>
       <c r="D32" s="1">
-        <v>1022255</v>
+        <v>1852183</v>
       </c>
       <c r="E32" s="1">
-        <v>0.13800000000000001</v>
+        <v>0.51800000000000002</v>
       </c>
       <c r="F32">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G32" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H32" s="1">
         <f t="shared" si="1"/>
-        <v>1.3800000000000001</v>
+        <v>0.51800000000000002</v>
       </c>
       <c r="I32" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J32" s="1">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="K32" s="1">
         <f t="shared" si="3"/>
-        <v>1.3800000000000001</v>
+        <v>1.036</v>
       </c>
     </row>
     <row r="33" spans="1:11">
       <c r="A33" s="1" t="s">
-        <v>90</v>
+        <v>23</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1">
         <v>1</v>
       </c>
       <c r="D33" s="1">
-        <v>1852183</v>
+        <v>1432565</v>
       </c>
       <c r="E33" s="1">
-        <v>0.51800000000000002</v>
+        <v>0.754</v>
       </c>
       <c r="F33">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G33" s="1">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H33" s="1">
         <f t="shared" si="1"/>
-        <v>0.51800000000000002</v>
+        <v>3.77</v>
       </c>
       <c r="I33" s="1">
         <v>2</v>
       </c>
       <c r="J33" s="1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K33" s="1">
         <f t="shared" si="3"/>
-        <v>1.036</v>
+        <v>3.77</v>
       </c>
     </row>
     <row r="34" spans="1:11">
       <c r="A34" s="1" t="s">
-        <v>23</v>
+        <v>133</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1">
         <v>1</v>
       </c>
       <c r="D34" s="1">
-        <v>1432565</v>
+        <v>2464666</v>
       </c>
       <c r="E34" s="1">
-        <v>0.754</v>
+        <v>11.92</v>
       </c>
       <c r="F34">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G34" s="1">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H34" s="1">
         <f t="shared" si="1"/>
-        <v>3.77</v>
+        <v>11.92</v>
       </c>
       <c r="I34" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J34" s="1">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K34" s="1">
         <f t="shared" si="3"/>
-        <v>3.77</v>
+        <v>11.92</v>
       </c>
     </row>
     <row r="35" spans="1:11">
-      <c r="A35" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1">
-        <v>1</v>
-      </c>
-      <c r="D35" s="1">
-        <v>2464666</v>
-      </c>
-      <c r="E35" s="1">
-        <v>11.92</v>
-      </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-      <c r="G35" s="1">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
       <c r="H35" s="1">
-        <f t="shared" si="1"/>
-        <v>11.92</v>
-      </c>
-      <c r="I35" s="1">
-        <v>1</v>
-      </c>
-      <c r="J35" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f>SUM(H3:H34)</f>
+        <v>63.407000000000018</v>
       </c>
       <c r="K35" s="1">
-        <f t="shared" si="3"/>
-        <v>11.92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11">
-      <c r="H36" s="1">
-        <f>SUM(H3:H35)</f>
-        <v>64.742500000000007</v>
-      </c>
-      <c r="K36" s="1">
-        <f>SUM(K3:K35)</f>
-        <v>87.99</v>
+        <f>SUM(K3:K34)</f>
+        <v>85.319000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change RH/temp sensor to STH21
</commit_message>
<xml_diff>
--- a/CaptorBoard.xlsx
+++ b/CaptorBoard.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="141">
   <si>
     <t>Reference</t>
   </si>
@@ -440,6 +440,9 @@
   </si>
   <si>
     <t>LED-3mm</t>
+  </si>
+  <si>
+    <t>SHT21</t>
   </si>
 </sst>
 </file>
@@ -1529,10 +1532,10 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2336,14 +2339,18 @@
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="1" t="s">
-        <v>58</v>
+        <v>140</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1">
         <v>1</v>
       </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
+      <c r="D22" s="1">
+        <v>1855468</v>
+      </c>
+      <c r="E22" s="1">
+        <v>3.79</v>
+      </c>
       <c r="F22">
         <v>1</v>
       </c>
@@ -2353,7 +2360,7 @@
       </c>
       <c r="H22" s="1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.79</v>
       </c>
       <c r="I22" s="1">
         <v>2</v>
@@ -2364,7 +2371,7 @@
       </c>
       <c r="K22" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>7.58</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -2818,11 +2825,11 @@
     <row r="35" spans="1:11">
       <c r="H35" s="1">
         <f>SUM(H3:H34)</f>
-        <v>63.407000000000018</v>
+        <v>67.197000000000017</v>
       </c>
       <c r="K35" s="1">
         <f>SUM(K3:K34)</f>
-        <v>85.319000000000003</v>
+        <v>92.899000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update bon and cost
</commit_message>
<xml_diff>
--- a/CaptorBoard.xlsx
+++ b/CaptorBoard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\philippe.fouquet\Documents\sources\perso\CaptorBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E90F59-43DB-4065-AEB2-B34444A0707D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2847D99-78E9-478E-85E4-1D158001E4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4665" yWindow="2070" windowWidth="21585" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31980" yWindow="2085" windowWidth="21585" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CaptorBoard" sheetId="1" r:id="rId1"/>
@@ -401,7 +401,7 @@
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -555,6 +555,12 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -899,7 +905,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -907,6 +913,8 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="8" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1849,8 +1857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1858,7 +1866,7 @@
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -1970,7 +1978,7 @@
         <f>C6*B$1</f>
         <v>40</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="7" t="s">
         <v>118</v>
       </c>
       <c r="F6" s="2">
@@ -1998,7 +2006,7 @@
         <f t="shared" ref="D7:D29" si="0">C7*B$1</f>
         <v>40</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="7" t="s">
         <v>96</v>
       </c>
       <c r="F7" s="2">
@@ -2026,7 +2034,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="7" t="s">
         <v>97</v>
       </c>
       <c r="F8" s="2">
@@ -2054,7 +2062,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="7" t="s">
         <v>98</v>
       </c>
       <c r="F9" s="2">
@@ -2082,7 +2090,7 @@
         <f t="shared" si="0"/>
         <v>140</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="7" t="s">
         <v>99</v>
       </c>
       <c r="F10" s="2">
@@ -2110,7 +2118,7 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="7" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="2">
@@ -2138,7 +2146,7 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E12" s="4" t="s">
+      <c r="E12" s="7" t="s">
         <v>101</v>
       </c>
       <c r="F12" s="2">
@@ -2166,7 +2174,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="7" t="s">
         <v>115</v>
       </c>
       <c r="F13" s="5">
@@ -2216,7 +2224,7 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="7" t="s">
         <v>113</v>
       </c>
       <c r="F15" s="2">
@@ -2290,7 +2298,7 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="7" t="s">
         <v>44</v>
       </c>
       <c r="F18" s="2">
@@ -2318,7 +2326,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="7" t="s">
         <v>49</v>
       </c>
       <c r="F19" s="2">
@@ -2346,7 +2354,7 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="E20" s="7" t="s">
         <v>102</v>
       </c>
       <c r="F20" s="2">
@@ -2374,7 +2382,7 @@
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="8" t="s">
         <v>106</v>
       </c>
       <c r="F21" s="2">
@@ -2402,7 +2410,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="E22" s="8" t="s">
         <v>107</v>
       </c>
       <c r="F22" s="2">
@@ -2430,7 +2438,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="8" t="s">
         <v>108</v>
       </c>
       <c r="F23" s="6">
@@ -2458,7 +2466,7 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="8" t="s">
         <v>110</v>
       </c>
       <c r="F24" s="2">
@@ -2486,7 +2494,7 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="8" t="s">
         <v>65</v>
       </c>
       <c r="F25" s="2">
@@ -2514,7 +2522,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E26" s="8" t="s">
         <v>69</v>
       </c>
       <c r="F26" s="5">
@@ -2542,7 +2550,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="8" t="s">
         <v>74</v>
       </c>
       <c r="F27" s="2">
@@ -2570,7 +2578,7 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="8" t="s">
         <v>103</v>
       </c>
       <c r="F28" s="2">
@@ -2598,7 +2606,7 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="8" t="s">
         <v>111</v>
       </c>
       <c r="F29" s="2">
@@ -2636,21 +2644,7 @@
       <c r="G37" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E7" r:id="rId1" display="https://www.mouser.fr/ProductDetail/KEMET/C1210C120J1HACTU?qs=W0yvOO0ixfEmRrcetHqPgA%3D%3D" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="E8" r:id="rId2" display="https://www.mouser.fr/ProductDetail/Samsung-Electro-Mechanics/CL32A226MOJNNNE?qs=X6jEic%2FHinDrCPX6SLC7PA%3D%3D" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-    <hyperlink ref="E9" r:id="rId3" display="https://www.mouser.fr/ProductDetail/Samsung-Electro-Mechanics/CL32B105KBHNNNE?qs=349EhDEZ59rXY4nCVEMdbA%3D%3D" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
-    <hyperlink ref="E10" r:id="rId4" display="https://www.mouser.fr/ProductDetail/Lite-On/LTST-C930KGKT?qs=qxhnwC4CwxkfAQj1wZIfSQ%3D%3D" xr:uid="{BAF6ED0D-6B67-4CB9-A15A-57C17B730A7D}"/>
-    <hyperlink ref="E11" r:id="rId5" display="https://www.mouser.fr/ProductDetail/onsemi/MRA4007T3G?qs=ZpPixqFcBtze9zNLkB8kog%3D%3D" xr:uid="{3C12269F-D067-44D8-BF0E-E945324B2D59}"/>
-    <hyperlink ref="E12" r:id="rId6" display="https://www.mouser.fr/ProductDetail/Comchip-Technology/1N4004T-G?qs=tw%252BuQ%2FB6PO3qoBZGQQOUiQ%3D%3D" xr:uid="{46C0D30D-8C70-445D-AC26-09F3459FE687}"/>
-    <hyperlink ref="E15" r:id="rId7" display="https://www.mouser.fr/ProductDetail/CUI-Devices/TB007-508-03BE?qs=sGAEpiMZZMvPvGwLNS671%2FDanv8Jav06cNprADDV8o%252BpBxzbBkYX8w%3D%3D" xr:uid="{A7C4017B-06A2-4C82-8958-B1BD625099E8}"/>
-    <hyperlink ref="E20" r:id="rId8" display="https://www.mouser.fr/ProductDetail/CUI-Devices/TB007-508-03BE?qs=sGAEpiMZZMvPvGwLNS671%2FDanv8Jav06cNprADDV8o%252BpBxzbBkYX8w%3D%3D" xr:uid="{C382A474-1EA4-4704-B536-3E0B482B9DB0}"/>
-    <hyperlink ref="E13" r:id="rId9" display="https://www.mouser.fr/ProductDetail/Littelfuse/0443001.DR?qs=PalBzRKzfntIMFnMK4x4WA%3D%3D" xr:uid="{D74FE405-09B9-43B0-A239-5B50E30DFAF9}"/>
-    <hyperlink ref="E6" r:id="rId10" display="https://www.mouser.fr/ProductDetail/KYOCERA-AVX/12101C104K4T2A?qs=46Fswce4YXnjVHFdHduUPA%3D%3D" xr:uid="{83E5B84C-90A6-4CA7-B636-ECB590866C53}"/>
-    <hyperlink ref="E18" r:id="rId11" display="https://www.mouser.fr/ProductDetail/Omron-Electronics/G5LE-1-DC5?qs=ImaqFqjHA4nKN7ETIjn3Lg%3D%3D" xr:uid="{FDE5AD49-7BE9-4F0B-BB1A-F37752447A47}"/>
-    <hyperlink ref="E19" r:id="rId12" display="https://www.mouser.fr/ProductDetail/MEAN-WELL/IRM-05-5?qs=WkdRfq4wf1OdYoHS8Am9VA%3D%3D" xr:uid="{1A607E26-14F6-4F81-B0A4-597AAB354767}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId13"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change somme manufacturer referance
</commit_message>
<xml_diff>
--- a/CaptorBoard.xlsx
+++ b/CaptorBoard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philippefouquet/Documents/Developpement/Electronique/CaptorBoard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3841B19F-1708-7543-A0CC-3113F367A5C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294FF1EA-B366-184A-8321-C293AB84A5A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="30280" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="33180" windowHeight="19780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CaptorBoard" sheetId="1" r:id="rId1"/>
@@ -259,7 +259,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>31354 En stock</t>
+          <t>31229 En stock</t>
         </r>
       </text>
     </comment>
@@ -307,7 +307,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>7870 En stock</t>
+          <t>7370 En stock</t>
         </r>
       </text>
     </comment>
@@ -323,14 +323,14 @@
           <t>Qty/Price Breaks (EUR):
   Qty  -  Unit€  -  Ext€
 ================
-     1   €0.28      €0.28
-    10   €0.19      €1.94
-   100   €0.10      €9.90
-   500   €0.07     €34.00
-  1000   €0.06     €60.00
-  2000   €0.06    €114.00
-  4000   €0.05    €204.00
-  8000   €0.05    €392.00</t>
+     1   €0.25      €0.25
+    10   €0.17      €1.71
+   100   €0.09      €8.60
+  1000   €0.05     €53.00
+  4000   €0.05    €200.00
+  8000   €0.04    €320.00
+ 24000   €0.04    €936.00
+100000   €0.04  €3,500.00</t>
         </r>
       </text>
     </comment>
@@ -356,7 +356,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>71647 En stock</t>
+          <t>66327 En stock</t>
         </r>
       </text>
     </comment>
@@ -406,7 +406,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>375502 En stock</t>
+          <t>363274 En stock</t>
         </r>
       </text>
     </comment>
@@ -451,11 +451,11 @@
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>80579 En stock</t>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>67499 En stock</t>
         </r>
       </text>
     </comment>
@@ -464,22 +464,121 @@
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Qty/Price Breaks (EUR):
-  Qty  -  Unit€  -  Ext€
-================
-     1   €0.34      €0.34
-    10   €0.18      €1.85
-   100   €0.09      €8.60
-   500   €0.08     €39.50
-  1000   €0.06     €62.00
-  1500   €0.06     €90.00
-  9000   €0.05    €423.00
- 24000   €0.04    €984.00
- 49500   €0.04  €1,881.00</t>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Qty/Price Breaks (EUR):
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  Qty  -  Unit€  -  Ext€
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">================
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">     1   €0.34      €0.34
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    10   €0.18      €1.85
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">   100   €0.09      €8.60
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">   500   €0.08     €39.50
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  1000   €0.06     €62.00
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  1500   €0.06     €90.00
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  9000   €0.05    €423.00
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> 24000   €0.04    €984.00
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> 49500   €0.04  €1,881.00</t>
         </r>
       </text>
     </comment>
@@ -505,7 +604,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>157760 En stock</t>
+          <t>146524 En stock</t>
         </r>
       </text>
     </comment>
@@ -555,7 +654,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>60400 En stock</t>
+          <t>61636 En stock</t>
         </r>
       </text>
     </comment>
@@ -601,11 +700,11 @@
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>2293 En stock</t>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2243 En stock</t>
         </r>
       </text>
     </comment>
@@ -614,16 +713,81 @@
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Qty/Price Breaks (EUR):
-  Qty  -  Unit€  -  Ext€
-================
-     1   €1.14      €1.14
-    10   €0.99      €9.90
-  1500   €0.99  €1,485.00</t>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Qty/Price Breaks (EUR):
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  Qty  -  Unit€  -  Ext€
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">================
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">     1   €1.13      €1.13
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    10   €0.92      €9.15
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">   100   €0.84     €84.00
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  1500   €0.84  €1,260.00
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  3000   €0.84  €2,508.00</t>
         </r>
       </text>
     </comment>
@@ -649,7 +813,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>14594 En stock</t>
+          <t>12242 En stock</t>
         </r>
       </text>
     </comment>
@@ -699,11 +863,289 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>5523 En stock</t>
+          <t>4434 En stock</t>
         </r>
       </text>
     </comment>
     <comment ref="J16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002C000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Qty/Price Breaks (EUR):
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  Qty  -  Unit€  -  Ext€
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">================
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">     1   €1.55      €1.55
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    10   €1.45     €14.50
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    25   €1.29     €32.25
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    50   €1.22     €61.00
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">   100   €1.16    €116.00
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">   250   €1.13    €282.50
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">   500   €1.06    €530.00</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002D000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Desc: Relais universels SPDT 5VDC Flux Protected</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002E000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>479 En stock</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002F000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Qty/Price Breaks (EUR):
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  Qty  -  Unit€  -  Ext€
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">================
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">     1   €6.67      €6.67
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">     5   €6.59     €32.95
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    10   €6.50     €65.00
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    25   €6.32    €158.00
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    60   €5.94    €356.40
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">   120   €5.75    €690.00
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">   300   €5.56  €1,668.00
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">   540   €5.49  €2,964.60
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  1020   €5.24  €5,344.80</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000030000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Desc: Modules d'alimentation CA/CC ac-dc, 5 W, 5 Vdc, single output, encapsulated PCB, 85~305 Vac</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000031000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>80273 En stock</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000032000000}">
       <text>
         <r>
           <rPr>
@@ -715,108 +1157,13 @@
           <t>Qty/Price Breaks (EUR):
   Qty  -  Unit€  -  Ext€
 ================
-     1   €1.55      €1.55
-    10   €1.45     €14.50
-    25   €1.29     €32.25
-    50   €1.22     €61.00
-   100   €1.19    €119.00</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002D000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Desc: Relais universels SPDT 5VDC Flux Protected</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002E000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>463 En stock</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002F000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Qty/Price Breaks (EUR):
-  Qty  -  Unit€  -  Ext€
-================
-     1   €6.67      €6.67
-     5   €6.59     €32.95
-    10   €6.50     €65.00
-    25   €6.32    €158.00
-    60   €5.94    €356.40
-   120   €5.75    €690.00
-   300   €5.56  €1,668.00
-   540   €5.49  €2,964.60
-  1020   €5.24  €5,344.80</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000030000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Desc: Modules d'alimentation CA/CC ac-dc, 5 W, 5 Vdc, single output, encapsulated PCB, 85~305 Vac</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000031000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>561 En stock</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="J18" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000032000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Qty/Price Breaks (EUR):
-  Qty  -  Unit€  -  Ext€
-================
-     1   €0.22      €0.22
-    10   €0.17      €1.75
-   100   €0.09      €9.30
-   500   €0.06     €30.50
-  1000   €0.04     €42.00
-  3000   €0.04    €114.00</t>
+     1   €0.27      €0.27
+    10   €0.22      €2.24
+   100   €0.12     €11.80
+   500   €0.08     €39.00
+  1000   €0.05     €54.00
+  3000   €0.05    €141.00
+  6000   €0.04    €270.00</t>
         </r>
       </text>
     </comment>
@@ -829,7 +1176,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Desc: MOSFET NFET SOT23 60V 380mA 2.5Ohms</t>
+          <t>Desc: MOSFET N-Channel</t>
         </r>
       </text>
     </comment>
@@ -898,18 +1245,81 @@
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Qty/Price Breaks (EUR):
-  Qty  -  Unit€  -  Ext€
-================
-     1   €0.72      €0.72
-    10   €0.54      €5.43
-   100   €0.32     €31.50
-  1000   €0.22    €223.00
-  4000   €0.22    €892.00</t>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Qty/Price Breaks (EUR):
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  Qty  -  Unit€  -  Ext€
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">================
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">     1   €0.72      €0.72
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">    10   €0.54      €5.43
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">   100   €0.32     €31.50
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  1000   €0.22    €223.00
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">  4000   €0.22    €892.00</t>
         </r>
       </text>
     </comment>
@@ -935,7 +1345,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>22055 En stock</t>
+          <t>21928 En stock</t>
         </r>
       </text>
     </comment>
@@ -978,11 +1388,11 @@
         <r>
           <rPr>
             <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>8857 En stock</t>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>8407 En stock</t>
         </r>
       </text>
     </comment>
@@ -1030,7 +1440,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>4641 En stock</t>
+          <t>3439 En stock</t>
         </r>
       </text>
     </comment>
@@ -1080,7 +1490,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>40832 En stock</t>
+          <t>37679 En stock</t>
         </r>
       </text>
     </comment>
@@ -1169,7 +1579,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>273 En stock</t>
+          <t>15584 En stock</t>
         </r>
       </text>
     </comment>
@@ -1185,15 +1595,15 @@
           <t>Qty/Price Breaks (EUR):
   Qty  -  Unit€  -  Ext€
 ================
-     1   €1.03      €1.03
-    10   €0.65      €6.51
-   100   €0.48     €48.00
-   500   €0.46    €229.00
-  1000   €0.37    €368.00
-  2000   €0.35    €700.00
-  5000   €0.34  €1,710.00
- 10000   €0.34  €3,350.00
- 25000   €0.33  €8,250.00</t>
+     1   €1.00      €1.00
+    10   €0.65      €6.47
+   100   €0.42     €42.50
+   500   €0.41    €207.00
+  1000   €0.33    €326.00
+  3000   €0.32    €960.00
+  5000   €0.31  €1,540.00
+ 10000   €0.30  €3,040.00
+ 25000   €0.29  €7,250.00</t>
         </r>
       </text>
     </comment>
@@ -1206,7 +1616,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Desc: Optocoupleurs de sortie triac et SCR 6Pin400V Optocoupler Zero Cross Triac Dr</t>
+          <t>Desc: Optocoupleurs de sortie triac et SCR DIP-6 ZERO TRIAC</t>
         </r>
       </text>
     </comment>
@@ -1219,7 +1629,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>28268 En stock</t>
+          <t>25407 En stock</t>
         </r>
       </text>
     </comment>
@@ -1453,7 +1863,7 @@
     <t>SOT-23</t>
   </si>
   <si>
-    <t>2N7002KT1G</t>
+    <t>2N7002E-7-F</t>
   </si>
   <si>
     <t>R1,R5,R7-R11,R14</t>
@@ -1534,7 +1944,7 @@
     <t>DIP-6_W7.62mm</t>
   </si>
   <si>
-    <t>MOC3041VM</t>
+    <t>MOC3041M</t>
   </si>
   <si>
     <t>Y1</t>
@@ -1594,7 +2004,7 @@
     <t>490-PSK-5D-5</t>
   </si>
   <si>
-    <t>863-2N7002KT1G</t>
+    <t>621-2N7002E-7-F</t>
   </si>
   <si>
     <t>791-RMC1/4-102JTE</t>
@@ -1618,7 +2028,7 @@
     <t>579-TC1264-3.3VDBTR</t>
   </si>
   <si>
-    <t>512-MOC3041VM</t>
+    <t>512-MOC3041-M</t>
   </si>
   <si>
     <t>428-201494-MC01</t>
@@ -1645,7 +2055,7 @@
     <t>Prj date:</t>
   </si>
   <si>
-    <t>2023 April 02, Sunday 15:11:16</t>
+    <t>2023 May 01, Monday 16:40:26</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -1660,7 +2070,7 @@
     <t>$ date:</t>
   </si>
   <si>
-    <t>2023-04-02 15:11:22</t>
+    <t>2023-05-01 16:40:50</t>
   </si>
   <si>
     <t>KiCost® v1.1.15</t>
@@ -1674,7 +2084,7 @@
     <numFmt numFmtId="164" formatCode="\€#,##0.00"/>
     <numFmt numFmtId="165" formatCode="\€#,##0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1748,6 +2158,12 @@
     <font>
       <sz val="8"/>
       <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -3314,7 +3730,7 @@
       <pane xSplit="7" ySplit="6" topLeftCell="H7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" outlineLevelCol="3" x14ac:dyDescent="0.2"/>
@@ -3345,7 +3761,7 @@
         <v>114</v>
       </c>
       <c r="G1" s="3">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -3358,7 +3774,7 @@
       </c>
       <c r="G2" s="4">
         <f>TotalCost/BoardQty</f>
-        <v>21.406000000000002</v>
+        <v>21.833999999999996</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.2">
@@ -3373,11 +3789,11 @@
       </c>
       <c r="G3" s="5">
         <f>SUM(G7:G27)</f>
-        <v>642.18000000000006</v>
+        <v>436.67999999999995</v>
       </c>
       <c r="L3" s="5">
         <f>SUM(L7:L27)</f>
-        <v>642.18000000000006</v>
+        <v>436.67999999999995</v>
       </c>
       <c r="M3" s="6" t="str">
         <f>(COUNTA(L7:L27)&amp;" of "&amp;ROWS(L7:L27)&amp;" parts found")</f>
@@ -3467,7 +3883,7 @@
       </c>
       <c r="E7" s="8">
         <f>CEILING(BoardQty*2,1)</f>
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F7" s="9">
         <f t="shared" ref="F7:F27" si="0">IF(MIN(J7)&lt;&gt;0,MIN(J7),"")</f>
@@ -3475,10 +3891,10 @@
       </c>
       <c r="G7" s="10">
         <f t="shared" ref="G7:G27" si="1">IF(AND(ISNUMBER(E7),ISNUMBER(F7)),E7*F7,"")</f>
-        <v>6.72</v>
+        <v>4.4800000000000004</v>
       </c>
       <c r="H7" s="8">
-        <v>31354</v>
+        <v>31229</v>
       </c>
       <c r="I7" s="8"/>
       <c r="J7" s="9">
@@ -3490,7 +3906,7 @@
       </c>
       <c r="L7" s="10">
         <f t="shared" ref="L7:L27" si="2">IFERROR(IF(I7="",E7,I7)*J7,"")</f>
-        <v>6.72</v>
+        <v>4.4800000000000004</v>
       </c>
       <c r="M7" s="8" t="s">
         <v>85</v>
@@ -3511,30 +3927,30 @@
       </c>
       <c r="E8" s="8">
         <f>CEILING(BoardQty*2,1)</f>
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F8" s="9">
         <f t="shared" si="0"/>
-        <v>0.19400000000000001</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="G8" s="10">
         <f t="shared" si="1"/>
-        <v>11.64</v>
+        <v>6.8400000000000007</v>
       </c>
       <c r="H8" s="8">
-        <v>7870</v>
+        <v>7370</v>
       </c>
       <c r="I8" s="8"/>
       <c r="J8" s="9">
-        <f>IFERROR(IF(OR(I8&gt;=K8,E8&gt;=K8),LOOKUP(IF(I8="",E8,I8),{0,1,10,100,500,1000,2000,4000,8000},{0,0.282,0.194,0.099,0.068,0.06,0.057,0.051,0.049}),"MOQ="&amp;K8),"")</f>
-        <v>0.19400000000000001</v>
+        <f>IFERROR(IF(OR(I8&gt;=K8,E8&gt;=K8),LOOKUP(IF(I8="",E8,I8),{0,1,10,100,1000,4000,8000,24000,100000},{0,0.254,0.171,0.086,0.053,0.05,0.04,0.039,0.035}),"MOQ="&amp;K8),"")</f>
+        <v>0.17100000000000001</v>
       </c>
       <c r="K8" s="8">
         <v>1</v>
       </c>
       <c r="L8" s="10">
         <f t="shared" si="2"/>
-        <v>11.64</v>
+        <v>6.8400000000000007</v>
       </c>
       <c r="M8" s="8" t="s">
         <v>86</v>
@@ -3555,7 +3971,7 @@
       </c>
       <c r="E9" s="8">
         <f>CEILING(BoardQty*1,1)</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F9" s="9">
         <f t="shared" si="0"/>
@@ -3563,10 +3979,10 @@
       </c>
       <c r="G9" s="10">
         <f t="shared" si="1"/>
-        <v>6.9</v>
+        <v>4.6000000000000005</v>
       </c>
       <c r="H9" s="8">
-        <v>71647</v>
+        <v>66327</v>
       </c>
       <c r="I9" s="8"/>
       <c r="J9" s="9">
@@ -3578,7 +3994,7 @@
       </c>
       <c r="L9" s="10">
         <f t="shared" si="2"/>
-        <v>6.9</v>
+        <v>4.6000000000000005</v>
       </c>
       <c r="M9" s="8" t="s">
         <v>87</v>
@@ -3599,7 +4015,7 @@
       </c>
       <c r="E10" s="8">
         <f>CEILING(BoardQty*1,1)</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F10" s="9">
         <f t="shared" si="0"/>
@@ -3607,10 +4023,10 @@
       </c>
       <c r="G10" s="10">
         <f t="shared" si="1"/>
-        <v>4.53</v>
+        <v>3.02</v>
       </c>
       <c r="H10" s="8">
-        <v>375502</v>
+        <v>363274</v>
       </c>
       <c r="I10" s="8"/>
       <c r="J10" s="9">
@@ -3622,7 +4038,7 @@
       </c>
       <c r="L10" s="10">
         <f t="shared" si="2"/>
-        <v>4.53</v>
+        <v>3.02</v>
       </c>
       <c r="M10" s="8" t="s">
         <v>88</v>
@@ -3643,7 +4059,7 @@
       </c>
       <c r="E11" s="8">
         <f>CEILING(BoardQty*7,1)</f>
-        <v>210</v>
+        <v>140</v>
       </c>
       <c r="F11" s="9">
         <f t="shared" si="0"/>
@@ -3651,10 +4067,10 @@
       </c>
       <c r="G11" s="10">
         <f t="shared" si="1"/>
-        <v>18.059999999999999</v>
+        <v>12.04</v>
       </c>
       <c r="H11" s="8">
-        <v>80579</v>
+        <v>67499</v>
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="9">
@@ -3666,7 +4082,7 @@
       </c>
       <c r="L11" s="10">
         <f t="shared" si="2"/>
-        <v>18.059999999999999</v>
+        <v>12.04</v>
       </c>
       <c r="M11" s="8" t="s">
         <v>89</v>
@@ -3687,7 +4103,7 @@
       </c>
       <c r="E12" s="8">
         <f>CEILING(BoardQty*2,1)</f>
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F12" s="9">
         <f t="shared" si="0"/>
@@ -3695,10 +4111,10 @@
       </c>
       <c r="G12" s="10">
         <f t="shared" si="1"/>
-        <v>10.379999999999999</v>
+        <v>6.92</v>
       </c>
       <c r="H12" s="8">
-        <v>157760</v>
+        <v>146524</v>
       </c>
       <c r="I12" s="8"/>
       <c r="J12" s="9">
@@ -3710,7 +4126,7 @@
       </c>
       <c r="L12" s="10">
         <f t="shared" si="2"/>
-        <v>10.379999999999999</v>
+        <v>6.92</v>
       </c>
       <c r="M12" s="8" t="s">
         <v>90</v>
@@ -3731,7 +4147,7 @@
       </c>
       <c r="E13" s="8">
         <f>CEILING(BoardQty*2,1)</f>
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F13" s="9">
         <f t="shared" si="0"/>
@@ -3739,10 +4155,10 @@
       </c>
       <c r="G13" s="10">
         <f t="shared" si="1"/>
-        <v>6.18</v>
+        <v>4.12</v>
       </c>
       <c r="H13" s="8">
-        <v>60400</v>
+        <v>61636</v>
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="9">
@@ -3754,7 +4170,7 @@
       </c>
       <c r="L13" s="10">
         <f t="shared" si="2"/>
-        <v>6.18</v>
+        <v>4.12</v>
       </c>
       <c r="M13" s="8" t="s">
         <v>91</v>
@@ -3775,30 +4191,30 @@
       </c>
       <c r="E14" s="8">
         <f>CEILING(BoardQty*1,1)</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F14" s="9">
         <f t="shared" si="0"/>
-        <v>0.99</v>
+        <v>0.91500000000000004</v>
       </c>
       <c r="G14" s="10">
         <f t="shared" si="1"/>
-        <v>29.7</v>
+        <v>18.3</v>
       </c>
       <c r="H14" s="8">
-        <v>2293</v>
+        <v>2243</v>
       </c>
       <c r="I14" s="8"/>
       <c r="J14" s="9">
-        <f>IFERROR(IF(OR(I14&gt;=K14,E14&gt;=K14),LOOKUP(IF(I14="",E14,I14),{0,1,10,1500},{0,1.14,0.99,0.99}),"MOQ="&amp;K14),"")</f>
-        <v>0.99</v>
+        <f>IFERROR(IF(OR(I14&gt;=K14,E14&gt;=K14),LOOKUP(IF(I14="",E14,I14),{0,1,10,100,1500,3000},{0,1.13,0.915,0.84,0.84,0.836}),"MOQ="&amp;K14),"")</f>
+        <v>0.91500000000000004</v>
       </c>
       <c r="K14" s="8">
         <v>1</v>
       </c>
       <c r="L14" s="10">
         <f t="shared" si="2"/>
-        <v>29.7</v>
+        <v>18.3</v>
       </c>
       <c r="M14" s="8" t="s">
         <v>92</v>
@@ -3819,7 +4235,7 @@
       </c>
       <c r="E15" s="8">
         <f>CEILING(BoardQty*3,1)</f>
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="F15" s="9">
         <f t="shared" si="0"/>
@@ -3827,10 +4243,10 @@
       </c>
       <c r="G15" s="10">
         <f t="shared" si="1"/>
-        <v>39.78</v>
+        <v>26.52</v>
       </c>
       <c r="H15" s="8">
-        <v>14594</v>
+        <v>12242</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="9">
@@ -3842,7 +4258,7 @@
       </c>
       <c r="L15" s="10">
         <f t="shared" si="2"/>
-        <v>39.78</v>
+        <v>26.52</v>
       </c>
       <c r="M15" s="8" t="s">
         <v>93</v>
@@ -3863,30 +4279,30 @@
       </c>
       <c r="E16" s="8">
         <f>CEILING(BoardQty*2,1)</f>
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F16" s="9">
         <f t="shared" si="0"/>
-        <v>1.22</v>
+        <v>1.29</v>
       </c>
       <c r="G16" s="10">
         <f t="shared" si="1"/>
-        <v>73.2</v>
+        <v>51.6</v>
       </c>
       <c r="H16" s="8">
-        <v>5523</v>
+        <v>4434</v>
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="9">
-        <f>IFERROR(IF(OR(I16&gt;=K16,E16&gt;=K16),LOOKUP(IF(I16="",E16,I16),{0,1,10,25,50,100},{0,1.55,1.45,1.29,1.22,1.19}),"MOQ="&amp;K16),"")</f>
-        <v>1.22</v>
+        <f>IFERROR(IF(OR(I16&gt;=K16,E16&gt;=K16),LOOKUP(IF(I16="",E16,I16),{0,1,10,25,50,100,250,500},{0,1.55,1.45,1.29,1.22,1.16,1.13,1.06}),"MOQ="&amp;K16),"")</f>
+        <v>1.29</v>
       </c>
       <c r="K16" s="8">
         <v>1</v>
       </c>
       <c r="L16" s="10">
         <f t="shared" si="2"/>
-        <v>73.2</v>
+        <v>51.6</v>
       </c>
       <c r="M16" s="8" t="s">
         <v>94</v>
@@ -3907,30 +4323,30 @@
       </c>
       <c r="E17" s="8">
         <f>CEILING(BoardQty*1,1)</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F17" s="9">
         <f t="shared" si="0"/>
-        <v>6.32</v>
+        <v>6.5</v>
       </c>
       <c r="G17" s="10">
         <f t="shared" si="1"/>
-        <v>189.60000000000002</v>
+        <v>130</v>
       </c>
       <c r="H17" s="8">
-        <v>463</v>
+        <v>479</v>
       </c>
       <c r="I17" s="8"/>
       <c r="J17" s="9">
         <f>IFERROR(IF(OR(I17&gt;=K17,E17&gt;=K17),LOOKUP(IF(I17="",E17,I17),{0,1,5,10,25,60,120,300,540,1020},{0,6.67,6.59,6.5,6.32,5.94,5.75,5.56,5.49,5.24}),"MOQ="&amp;K17),"")</f>
-        <v>6.32</v>
+        <v>6.5</v>
       </c>
       <c r="K17" s="8">
         <v>1</v>
       </c>
       <c r="L17" s="10">
         <f t="shared" si="2"/>
-        <v>189.60000000000002</v>
+        <v>130</v>
       </c>
       <c r="M17" s="8" t="s">
         <v>95</v>
@@ -3951,30 +4367,30 @@
       </c>
       <c r="E18" s="8">
         <f>CEILING(BoardQty*2,1)</f>
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F18" s="9">
         <f t="shared" si="0"/>
-        <v>0.17499999999999999</v>
+        <v>0.224</v>
       </c>
       <c r="G18" s="10">
         <f t="shared" si="1"/>
-        <v>10.5</v>
+        <v>8.9600000000000009</v>
       </c>
       <c r="H18" s="8">
-        <v>561</v>
+        <v>80273</v>
       </c>
       <c r="I18" s="8"/>
       <c r="J18" s="9">
-        <f>IFERROR(IF(OR(I18&gt;=K18,E18&gt;=K18),LOOKUP(IF(I18="",E18,I18),{0,1,10,100,500,1000,3000},{0,0.216,0.175,0.093,0.061,0.042,0.038}),"MOQ="&amp;K18),"")</f>
-        <v>0.17499999999999999</v>
+        <f>IFERROR(IF(OR(I18&gt;=K18,E18&gt;=K18),LOOKUP(IF(I18="",E18,I18),{0,1,10,100,500,1000,3000,6000},{0,0.273,0.224,0.118,0.078,0.054,0.047,0.045}),"MOQ="&amp;K18),"")</f>
+        <v>0.224</v>
       </c>
       <c r="K18" s="8">
         <v>1</v>
       </c>
       <c r="L18" s="10">
         <f t="shared" si="2"/>
-        <v>10.5</v>
+        <v>8.9600000000000009</v>
       </c>
       <c r="M18" s="8" t="s">
         <v>96</v>
@@ -3995,7 +4411,7 @@
       </c>
       <c r="E19" s="8">
         <f>CEILING(BoardQty*8,1)</f>
-        <v>240</v>
+        <v>160</v>
       </c>
       <c r="F19" s="9">
         <f t="shared" si="0"/>
@@ -4003,7 +4419,7 @@
       </c>
       <c r="G19" s="10">
         <f t="shared" si="1"/>
-        <v>7.68</v>
+        <v>5.12</v>
       </c>
       <c r="H19" s="8">
         <v>7800</v>
@@ -4018,7 +4434,7 @@
       </c>
       <c r="L19" s="10">
         <f t="shared" si="2"/>
-        <v>7.68</v>
+        <v>5.12</v>
       </c>
       <c r="M19" s="8" t="s">
         <v>97</v>
@@ -4039,7 +4455,7 @@
       </c>
       <c r="E20" s="8">
         <f>CEILING(BoardQty*1,1)</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F20" s="9">
         <f t="shared" si="0"/>
@@ -4047,7 +4463,7 @@
       </c>
       <c r="G20" s="10">
         <f t="shared" si="1"/>
-        <v>16.290000000000003</v>
+        <v>10.860000000000001</v>
       </c>
       <c r="H20" s="8">
         <v>7700</v>
@@ -4062,7 +4478,7 @@
       </c>
       <c r="L20" s="10">
         <f t="shared" si="2"/>
-        <v>16.290000000000003</v>
+        <v>10.860000000000001</v>
       </c>
       <c r="M20" s="8" t="s">
         <v>98</v>
@@ -4083,7 +4499,7 @@
       </c>
       <c r="E21" s="8">
         <f>CEILING(BoardQty*3,1)</f>
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="F21" s="9">
         <f t="shared" si="0"/>
@@ -4091,10 +4507,10 @@
       </c>
       <c r="G21" s="10">
         <f t="shared" si="1"/>
-        <v>9.5399999999999991</v>
+        <v>6.3599999999999994</v>
       </c>
       <c r="H21" s="8">
-        <v>22055</v>
+        <v>21928</v>
       </c>
       <c r="I21" s="8"/>
       <c r="J21" s="9">
@@ -4106,7 +4522,7 @@
       </c>
       <c r="L21" s="10">
         <f t="shared" si="2"/>
-        <v>9.5399999999999991</v>
+        <v>6.3599999999999994</v>
       </c>
       <c r="M21" s="8" t="s">
         <v>99</v>
@@ -4127,7 +4543,7 @@
       </c>
       <c r="E22" s="8">
         <f>CEILING(BoardQty*2,1)</f>
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F22" s="9">
         <f t="shared" si="0"/>
@@ -4135,10 +4551,10 @@
       </c>
       <c r="G22" s="10">
         <f t="shared" si="1"/>
-        <v>8.16</v>
+        <v>5.44</v>
       </c>
       <c r="H22" s="8">
-        <v>8857</v>
+        <v>8407</v>
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="9">
@@ -4150,7 +4566,7 @@
       </c>
       <c r="L22" s="10">
         <f t="shared" si="2"/>
-        <v>8.16</v>
+        <v>5.44</v>
       </c>
       <c r="M22" s="8" t="s">
         <v>100</v>
@@ -4171,7 +4587,7 @@
       </c>
       <c r="E23" s="8">
         <f>CEILING(BoardQty*2,1)</f>
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F23" s="9">
         <f t="shared" si="0"/>
@@ -4179,10 +4595,10 @@
       </c>
       <c r="G23" s="10">
         <f t="shared" si="1"/>
-        <v>32.1</v>
+        <v>21.400000000000002</v>
       </c>
       <c r="H23" s="8">
-        <v>4641</v>
+        <v>3439</v>
       </c>
       <c r="I23" s="8"/>
       <c r="J23" s="9">
@@ -4194,7 +4610,7 @@
       </c>
       <c r="L23" s="10">
         <f t="shared" si="2"/>
-        <v>32.1</v>
+        <v>21.400000000000002</v>
       </c>
       <c r="M23" s="8" t="s">
         <v>101</v>
@@ -4215,7 +4631,7 @@
       </c>
       <c r="E24" s="8">
         <f>CEILING(BoardQty*1,1)</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F24" s="9">
         <f t="shared" si="0"/>
@@ -4223,10 +4639,10 @@
       </c>
       <c r="G24" s="10">
         <f t="shared" si="1"/>
-        <v>84.6</v>
+        <v>56.4</v>
       </c>
       <c r="H24" s="8">
-        <v>40832</v>
+        <v>37679</v>
       </c>
       <c r="I24" s="8"/>
       <c r="J24" s="9">
@@ -4238,7 +4654,7 @@
       </c>
       <c r="L24" s="10">
         <f t="shared" si="2"/>
-        <v>84.6</v>
+        <v>56.4</v>
       </c>
       <c r="M24" s="8" t="s">
         <v>102</v>
@@ -4259,15 +4675,15 @@
       </c>
       <c r="E25" s="8">
         <f>CEILING(BoardQty*1,1)</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F25" s="9">
         <f t="shared" si="0"/>
-        <v>0.76800000000000002</v>
+        <v>0.90700000000000003</v>
       </c>
       <c r="G25" s="10">
         <f t="shared" si="1"/>
-        <v>23.04</v>
+        <v>18.14</v>
       </c>
       <c r="H25" s="8">
         <v>3000</v>
@@ -4275,14 +4691,14 @@
       <c r="I25" s="8"/>
       <c r="J25" s="9">
         <f>IFERROR(IF(OR(I25&gt;=K25,E25&gt;=K25),LOOKUP(IF(I25="",E25,I25),{0,1,10,25,100,4000},{0,0.912,0.907,0.768,0.708,0.708}),"MOQ="&amp;K25),"")</f>
-        <v>0.76800000000000002</v>
+        <v>0.90700000000000003</v>
       </c>
       <c r="K25" s="8">
         <v>1</v>
       </c>
       <c r="L25" s="10">
         <f t="shared" si="2"/>
-        <v>23.04</v>
+        <v>18.14</v>
       </c>
       <c r="M25" s="8" t="s">
         <v>103</v>
@@ -4303,30 +4719,30 @@
       </c>
       <c r="E26" s="8">
         <f>CEILING(BoardQty*2,1)</f>
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="F26" s="9">
         <f t="shared" si="0"/>
-        <v>0.65100000000000002</v>
+        <v>0.64700000000000002</v>
       </c>
       <c r="G26" s="10">
         <f t="shared" si="1"/>
-        <v>39.06</v>
+        <v>25.880000000000003</v>
       </c>
       <c r="H26" s="8">
-        <v>273</v>
+        <v>15584</v>
       </c>
       <c r="I26" s="8"/>
       <c r="J26" s="9">
-        <f>IFERROR(IF(OR(I26&gt;=K26,E26&gt;=K26),LOOKUP(IF(I26="",E26,I26),{0,1,10,100,500,1000,2000,5000,10000,25000},{0,1.03,0.651,0.48,0.458,0.368,0.35,0.342,0.335,0.33}),"MOQ="&amp;K26),"")</f>
-        <v>0.65100000000000002</v>
+        <f>IFERROR(IF(OR(I26&gt;=K26,E26&gt;=K26),LOOKUP(IF(I26="",E26,I26),{0,1,10,100,500,1000,3000,5000,10000,25000},{0,0.996,0.647,0.425,0.414,0.326,0.32,0.308,0.304,0.29}),"MOQ="&amp;K26),"")</f>
+        <v>0.64700000000000002</v>
       </c>
       <c r="K26" s="8">
         <v>1</v>
       </c>
       <c r="L26" s="10">
         <f t="shared" si="2"/>
-        <v>39.06</v>
+        <v>25.880000000000003</v>
       </c>
       <c r="M26" s="8" t="s">
         <v>104</v>
@@ -4347,7 +4763,7 @@
       </c>
       <c r="E27" s="8">
         <f>CEILING(BoardQty*1,1)</f>
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F27" s="9">
         <f t="shared" si="0"/>
@@ -4355,10 +4771,10 @@
       </c>
       <c r="G27" s="10">
         <f t="shared" si="1"/>
-        <v>14.52</v>
+        <v>9.68</v>
       </c>
       <c r="H27" s="8">
-        <v>28268</v>
+        <v>25407</v>
       </c>
       <c r="I27" s="8"/>
       <c r="J27" s="9">
@@ -4370,7 +4786,7 @@
       </c>
       <c r="L27" s="10">
         <f t="shared" si="2"/>
-        <v>14.52</v>
+        <v>9.68</v>
       </c>
       <c r="M27" s="8" t="s">
         <v>105</v>

</xml_diff>